<commit_message>
add hold and buy to performance
</commit_message>
<xml_diff>
--- a/data/output/backtest_Close_BTC.xlsx
+++ b/data/output/backtest_Close_BTC.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H143"/>
+  <dimension ref="A1:I143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>valeur_crypto</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>valeur_portefeuille_buy_and_hold</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -508,6 +513,9 @@
       <c r="H2" t="n">
         <v>19319.77</v>
       </c>
+      <c r="I2" t="n">
+        <v>10013.94881328482</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -516,7 +524,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0006139511933795916</v>
+        <v>0.0006138469469600949</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -542,6 +550,9 @@
       <c r="H3" t="n">
         <v>21360.11</v>
       </c>
+      <c r="I3" t="n">
+        <v>11019.31162108887</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -550,7 +561,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.06152841315326185</v>
+        <v>0.06152842560246263</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -576,6 +587,9 @@
       <c r="H4" t="n">
         <v>22395.74</v>
       </c>
+      <c r="I4" t="n">
+        <v>11541.02752277414</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -584,7 +598,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.05214928615285963</v>
+        <v>0.05214948232460692</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -610,6 +624,9 @@
       <c r="H5" t="n">
         <v>20173.57</v>
       </c>
+      <c r="I5" t="n">
+        <v>10335.01980291704</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -618,7 +635,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.04688653162444112</v>
+        <v>-0.04688672676649652</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -644,6 +661,9 @@
       <c r="H6" t="n">
         <v>20226.71</v>
       </c>
+      <c r="I6" t="n">
+        <v>10362.20789513099</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -652,7 +672,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.01992861013985703</v>
+        <v>-0.01992836523031372</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -678,6 +698,9 @@
       <c r="H7" t="n">
         <v>19701.88</v>
       </c>
+      <c r="I7" t="n">
+        <v>10089.78601396135</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -686,7 +709,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.03630056167199491</v>
+        <v>-0.03630076626129508</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -712,6 +735,9 @@
       <c r="H8" t="n">
         <v>19803.3</v>
       </c>
+      <c r="I8" t="n">
+        <v>10141.59230091841</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -720,7 +746,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.006182424548773824</v>
+        <v>-0.006182425508914235</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -746,6 +772,9 @@
       <c r="H9" t="n">
         <v>19537.02</v>
       </c>
+      <c r="I9" t="n">
+        <v>10004.30086863715</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -754,7 +783,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.006602915185629499</v>
+        <v>-0.006602968488977012</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -780,6 +809,9 @@
       <c r="H10" t="n">
         <v>18875</v>
       </c>
+      <c r="I10" t="n">
+        <v>9659.424283789327</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -788,7 +820,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.02136562001574127</v>
+        <v>-0.02136562453104141</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -814,6 +846,9 @@
       <c r="H11" t="n">
         <v>18461.36</v>
       </c>
+      <c r="I11" t="n">
+        <v>9445.386935685978</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -822,7 +857,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.01742774722772289</v>
+        <v>-0.01742764230501948</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -848,6 +883,9 @@
       <c r="H12" t="n">
         <v>19401.63</v>
       </c>
+      <c r="I12" t="n">
+        <v>9914.607160358497</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -856,7 +894,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.02946968185690224</v>
+        <v>0.02946957949093765</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -882,6 +920,9 @@
       <c r="H13" t="n">
         <v>19289.91</v>
       </c>
+      <c r="I13" t="n">
+        <v>9857.35107852255</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -890,7 +931,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.02028800547912368</v>
+        <v>0.02028816482165219</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -916,6 +957,9 @@
       <c r="H14" t="n">
         <v>19227.82</v>
       </c>
+      <c r="I14" t="n">
+        <v>9825.571248371789</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -924,7 +968,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.004594878475963071</v>
+        <v>0.004594878712980588</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -950,6 +994,9 @@
       <c r="H15" t="n">
         <v>19079.13</v>
       </c>
+      <c r="I15" t="n">
+        <v>9749.294148465651</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -958,7 +1005,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.00796211004945846</v>
+        <v>-0.007962266088021863</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -984,6 +1031,9 @@
       <c r="H16" t="n">
         <v>19412.82</v>
       </c>
+      <c r="I16" t="n">
+        <v>9918.333309385553</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -992,7 +1042,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.002646513878531209</v>
+        <v>0.002646617904192183</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1018,6 +1068,9 @@
       <c r="H17" t="n">
         <v>19591.51</v>
       </c>
+      <c r="I17" t="n">
+        <v>10009.21139283825</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1026,7 +1079,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.01477182908523034</v>
+        <v>0.01477172864263032</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1052,6 +1105,9 @@
       <c r="H18" t="n">
         <v>19422.61</v>
       </c>
+      <c r="I18" t="n">
+        <v>9922.547058703403</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1060,7 +1116,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.005116773069479663</v>
+        <v>-0.005116722874085156</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1086,6 +1142,9 @@
       <c r="H19" t="n">
         <v>19629.08</v>
       </c>
+      <c r="I19" t="n">
+        <v>10027.47093682329</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1094,7 +1153,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.008906010677121046</v>
+        <v>0.008906113614404632</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1120,6 +1179,9 @@
       <c r="H20" t="n">
         <v>20337.82</v>
       </c>
+      <c r="I20" t="n">
+        <v>10383.14600030795</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1128,7 +1190,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.02093312319408014</v>
+        <v>0.02093297504097436</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1154,6 +1216,9 @@
       <c r="H21" t="n">
         <v>20158.26</v>
       </c>
+      <c r="I21" t="n">
+        <v>10291.06746261975</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1162,7 +1227,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.005086278783874576</v>
+        <v>0.00508627979317211</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1188,6 +1253,9 @@
       <c r="H22" t="n">
         <v>19960.67</v>
       </c>
+      <c r="I22" t="n">
+        <v>10189.69743797309</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1196,7 +1264,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.005924217840890478</v>
+        <v>-0.00592431857048048</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1222,6 +1290,9 @@
       <c r="H23" t="n">
         <v>19530.09</v>
       </c>
+      <c r="I23" t="n">
+        <v>9967.485771263066</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1230,7 +1301,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.01449288376219471</v>
+        <v>-0.01449278711531932</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1256,6 +1327,9 @@
       <c r="H24" t="n">
         <v>19131.87</v>
       </c>
+      <c r="I24" t="n">
+        <v>9762.147368345386</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1264,7 +1338,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.02739012349140069</v>
+        <v>-0.02739007719521958</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1290,6 +1364,9 @@
       <c r="H25" t="n">
         <v>19060</v>
       </c>
+      <c r="I25" t="n">
+        <v>9725.406231577499</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1298,7 +1375,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.004555389673498667</v>
+        <v>-0.004555390384473057</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1324,6 +1401,9 @@
       <c r="H26" t="n">
         <v>19155.53</v>
       </c>
+      <c r="I26" t="n">
+        <v>9774.028872295068</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1332,7 +1412,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.00210477024987199</v>
+        <v>0.002104718545581363</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1358,6 +1438,9 @@
       <c r="H27" t="n">
         <v>19375.13</v>
       </c>
+      <c r="I27" t="n">
+        <v>9885.441445078804</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1366,7 +1449,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.005994534940302998</v>
+        <v>0.005994587906439364</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1392,6 +1475,9 @@
       <c r="H28" t="n">
         <v>19176.93</v>
       </c>
+      <c r="I28" t="n">
+        <v>9783.796461300119</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1400,7 +1486,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.001679456952427216</v>
+        <v>0.001679560483630382</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1426,6 +1512,9 @@
       <c r="H29" t="n">
         <v>19549.86</v>
       </c>
+      <c r="I29" t="n">
+        <v>9972.233664795238</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1434,7 +1523,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.01257060957335732</v>
+        <v>0.01257061021838268</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1460,6 +1549,9 @@
       <c r="H30" t="n">
         <v>19327.44</v>
       </c>
+      <c r="I30" t="n">
+        <v>9858.128600329792</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1468,7 +1560,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.007766135163812748</v>
+        <v>-0.007766238337204356</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1494,6 +1586,9 @@
       <c r="H31" t="n">
         <v>19123.97</v>
       </c>
+      <c r="I31" t="n">
+        <v>9753.7968138741</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1502,7 +1597,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.00858761550875542</v>
+        <v>-0.00858756500723068</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1528,6 +1623,9 @@
       <c r="H32" t="n">
         <v>19041.92</v>
       </c>
+      <c r="I32" t="n">
+        <v>9711.858828856122</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1536,7 +1634,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.009682597273567239</v>
+        <v>-0.00968254594673823</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1562,6 +1660,9 @@
       <c r="H33" t="n">
         <v>19164.37</v>
       </c>
+      <c r="I33" t="n">
+        <v>9774.111467645736</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1570,7 +1671,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.0003147480027134719</v>
+        <v>0.0003146433812766247</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1596,6 +1697,9 @@
       <c r="H34" t="n">
         <v>19329.72</v>
       </c>
+      <c r="I34" t="n">
+        <v>9858.080683239656</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1604,7 +1708,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.008503606628471161</v>
+        <v>0.008503556081565833</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1630,6 +1734,9 @@
       <c r="H35" t="n">
         <v>20080.07</v>
       </c>
+      <c r="I35" t="n">
+        <v>10233.5155619498</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1638,7 +1745,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.03792225184742826</v>
+        <v>0.03792210973251109</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1664,6 +1771,9 @@
       <c r="H36" t="n">
         <v>20771.59</v>
       </c>
+      <c r="I36" t="n">
+        <v>10580.00609489213</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1672,7 +1782,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.03280882286863829</v>
+        <v>0.03280907582040626</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1698,6 +1808,9 @@
       <c r="H37" t="n">
         <v>20295.11</v>
       </c>
+      <c r="I37" t="n">
+        <v>10334.48417391186</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1706,7 +1819,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-0.003937735766957218</v>
+        <v>-0.003937736148355242</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1732,6 +1845,9 @@
       <c r="H38" t="n">
         <v>20591.84</v>
       </c>
+      <c r="I38" t="n">
+        <v>10484.48828660941</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1740,7 +1856,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-0.001791951715237161</v>
+        <v>-0.001792049111680072</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1766,6 +1882,9 @@
       <c r="H39" t="n">
         <v>20490.74</v>
       </c>
+      <c r="I39" t="n">
+        <v>10432.88568981345</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1774,7 +1893,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.0004081534116728847</v>
+        <v>0.000408153491019192</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1800,6 +1919,9 @@
       <c r="H40" t="n">
         <v>20483.62</v>
       </c>
+      <c r="I40" t="n">
+        <v>10429.25990301121</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1808,7 +1930,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-0.01982575314808344</v>
+        <v>-0.01982575703997647</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1834,6 +1956,9 @@
       <c r="H41" t="n">
         <v>20151.84</v>
       </c>
+      <c r="I41" t="n">
+        <v>10258.95068322331</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1842,7 +1967,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-0.01910767868027108</v>
+        <v>-0.0191075814639472</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1868,6 +1993,9 @@
       <c r="H42" t="n">
         <v>20207.82</v>
       </c>
+      <c r="I42" t="n">
+        <v>10287.40961610498</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1876,7 +2004,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-0.005841636912469639</v>
+        <v>-0.005841637504442332</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1902,6 +2030,9 @@
       <c r="H43" t="n">
         <v>21148.52</v>
       </c>
+      <c r="I43" t="n">
+        <v>10755.48951559579</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1910,7 +2041,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.04350320782523909</v>
+        <v>0.04350330945818648</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1936,6 +2067,9 @@
       <c r="H44" t="n">
         <v>20591.13</v>
       </c>
+      <c r="I44" t="n">
+        <v>10468.2154872251</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1944,7 +2078,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-0.01385643135569303</v>
+        <v>-0.01385653001977616</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1970,6 +2104,9 @@
       <c r="H45" t="n">
         <v>18547.23</v>
       </c>
+      <c r="I45" t="n">
+        <v>9373.868776306044</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1978,7 +2115,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>-0.07985570324950864</v>
+        <v>-0.07985571145152903</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2004,6 +2141,9 @@
       <c r="H46" t="n">
         <v>15922.81</v>
       </c>
+      <c r="I46" t="n">
+        <v>7943.718432911791</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2012,7 +2152,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-0.1477979236897742</v>
+        <v>-0.147797878767463</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2038,6 +2178,9 @@
       <c r="H47" t="n">
         <v>17601.15</v>
       </c>
+      <c r="I47" t="n">
+        <v>8739.770916321771</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2046,7 +2189,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.01421707381032178</v>
+        <v>0.01421689147663585</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2072,6 +2215,9 @@
       <c r="H48" t="n">
         <v>17070.31</v>
       </c>
+      <c r="I48" t="n">
+        <v>8472.128160073413</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2080,7 +2226,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.006356252559591269</v>
+        <v>0.006356375472220677</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2106,6 +2252,9 @@
       <c r="H49" t="n">
         <v>16619.46</v>
       </c>
+      <c r="I49" t="n">
+        <v>8245.359795394152</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2114,7 +2263,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-0.009377087567214559</v>
+        <v>-0.009377149964747034</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2140,6 +2289,9 @@
       <c r="H50" t="n">
         <v>16900.57</v>
       </c>
+      <c r="I50" t="n">
+        <v>8383.659637785486</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2148,7 +2300,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.005238489791871359</v>
+        <v>0.005238368883798472</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2174,6 +2326,9 @@
       <c r="H51" t="n">
         <v>16662.76</v>
       </c>
+      <c r="I51" t="n">
+        <v>8264.854294987503</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2182,7 +2337,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-0.02029799658321529</v>
+        <v>-0.02029794064702983</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -2208,6 +2363,9 @@
       <c r="H52" t="n">
         <v>16692.56</v>
       </c>
+      <c r="I52" t="n">
+        <v>8279.622117542905</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2216,7 +2374,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.004535999001729962</v>
+        <v>0.004536062029579568</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -2242,6 +2400,9 @@
       <c r="H53" t="n">
         <v>16700.45</v>
       </c>
+      <c r="I53" t="n">
+        <v>8283.534686054887</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2250,7 +2411,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.005419552172616804</v>
+        <v>0.005419553176341907</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -2276,6 +2437,9 @@
       <c r="H54" t="n">
         <v>15781.29</v>
       </c>
+      <c r="I54" t="n">
+        <v>7814.59878387804</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2284,7 +2448,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.0450257620898924</v>
+        <v>-0.04502589940245727</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2310,6 +2474,9 @@
       <c r="H55" t="n">
         <v>16226.94</v>
       </c>
+      <c r="I55" t="n">
+        <v>8032.217877841495</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2318,7 +2485,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.006819837120012551</v>
+        <v>0.006819967239302116</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -2344,6 +2511,9 @@
       <c r="H56" t="n">
         <v>16603.11</v>
       </c>
+      <c r="I56" t="n">
+        <v>8216.293847118379</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2352,7 +2522,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.02987235948570799</v>
+        <v>0.02987242721610883</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -2378,6 +2548,9 @@
       <c r="H57" t="n">
         <v>16598.95</v>
       </c>
+      <c r="I57" t="n">
+        <v>8214.234951821943</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2386,7 +2559,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.0310831415252526</v>
+        <v>0.03108308514259939</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -2412,6 +2585,9 @@
       <c r="H58" t="n">
         <v>16522.14</v>
       </c>
+      <c r="I58" t="n">
+        <v>8176.136174413093</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2420,7 +2596,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-0.0017387455770006</v>
+        <v>-0.001738685603724477</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -2446,6 +2622,9 @@
       <c r="H59" t="n">
         <v>16212.91</v>
       </c>
+      <c r="I59" t="n">
+        <v>8021.66066280914</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2454,7 +2633,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-0.03353063423974589</v>
+        <v>-0.03353070069447384</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -2480,6 +2659,9 @@
       <c r="H60" t="n">
         <v>16442.53</v>
       </c>
+      <c r="I60" t="n">
+        <v>8134.472744315395</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2488,7 +2670,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-0.009099558301240762</v>
+        <v>-0.009099497097782461</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -2514,6 +2696,9 @@
       <c r="H61" t="n">
         <v>17163.64</v>
       </c>
+      <c r="I61" t="n">
+        <v>8483.619949329324</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2522,7 +2707,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.03510253127685203</v>
+        <v>0.03510229264497333</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -2548,6 +2733,9 @@
       <c r="H62" t="n">
         <v>16977.37</v>
       </c>
+      <c r="I62" t="n">
+        <v>8391.047435049451</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2556,7 +2744,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-0.008120999545745633</v>
+        <v>-0.008120757564272552</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -2582,6 +2770,9 @@
       <c r="H63" t="n">
         <v>17092.74</v>
       </c>
+      <c r="I63" t="n">
+        <v>8447.876065354347</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2590,7 +2781,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.01138788313199512</v>
+        <v>0.01138770288412871</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -2616,6 +2807,9 @@
       <c r="H64" t="n">
         <v>16966.35</v>
       </c>
+      <c r="I64" t="n">
+        <v>8385.177269990489</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2624,7 +2818,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-0.01389591733660467</v>
+        <v>-0.01389573739630023</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -2650,6 +2844,9 @@
       <c r="H65" t="n">
         <v>17088.96</v>
       </c>
+      <c r="I65" t="n">
+        <v>8445.556166985829</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2658,7 +2855,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.004765545071014898</v>
+        <v>0.004765423454299977</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -2684,6 +2881,9 @@
       <c r="H66" t="n">
         <v>16836.64</v>
       </c>
+      <c r="I66" t="n">
+        <v>8319.927024060547</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2692,7 +2892,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>-0.01057509972410031</v>
+        <v>-0.01057497882278291</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2718,6 +2918,9 @@
       <c r="H67" t="n">
         <v>17224.1</v>
       </c>
+      <c r="I67" t="n">
+        <v>8509.222851776227</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2726,7 +2929,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.01599008297881532</v>
+        <v>0.01599020647839566</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2752,6 +2955,9 @@
       <c r="H68" t="n">
         <v>17128.56</v>
       </c>
+      <c r="I68" t="n">
+        <v>8461.891830112809</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2760,7 +2966,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.00290230396736213</v>
+        <v>0.002902061590788207</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2786,6 +2992,9 @@
       <c r="H69" t="n">
         <v>17209.83</v>
       </c>
+      <c r="I69" t="n">
+        <v>8501.94608036003</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2794,7 +3003,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.01014394516542616</v>
+        <v>0.01014394761165072</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2820,6 +3029,9 @@
       <c r="H70" t="n">
         <v>17774.7</v>
       </c>
+      <c r="I70" t="n">
+        <v>8776.519538297502</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2828,7 +3040,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.01875360881318322</v>
+        <v>0.01875378987535825</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2854,6 +3066,9 @@
       <c r="H71" t="n">
         <v>17803.15</v>
       </c>
+      <c r="I71" t="n">
+        <v>8790.555913968672</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2862,7 +3077,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.01331837706614714</v>
+        <v>0.01331820357692948</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2888,6 +3103,9 @@
       <c r="H72" t="n">
         <v>17356.34</v>
       </c>
+      <c r="I72" t="n">
+        <v>8567.121515787678</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2896,7 +3114,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>-0.01221503114234501</v>
+        <v>-0.01221526921111149</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2922,6 +3140,9 @@
       <c r="H73" t="n">
         <v>16632.12</v>
       </c>
+      <c r="I73" t="n">
+        <v>8201.97287458458</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2930,7 +3151,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-0.0453946199526527</v>
+        <v>-0.04539433412887739</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2956,6 +3177,9 @@
       <c r="H74" t="n">
         <v>16438.88</v>
       </c>
+      <c r="I74" t="n">
+        <v>8106.120479624212</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2964,7 +3188,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-0.02569796228988785</v>
+        <v>-0.02569790395934568</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2990,6 +3214,9 @@
       <c r="H75" t="n">
         <v>16895.56</v>
       </c>
+      <c r="I75" t="n">
+        <v>8328.241188912458</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2998,7 +3225,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.01941489140600972</v>
+        <v>0.01941483191194671</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -3024,6 +3251,9 @@
       <c r="H76" t="n">
         <v>16824.67</v>
       </c>
+      <c r="I76" t="n">
+        <v>8293.224233947596</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3032,7 +3262,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.007408880558280373</v>
+        <v>0.007409066324184366</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -3058,6 +3288,9 @@
       <c r="H77" t="n">
         <v>16821.43</v>
       </c>
+      <c r="I77" t="n">
+        <v>8291.627017830366</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3066,7 +3299,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.007725657854152246</v>
+        <v>0.007725413886689125</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -3092,6 +3325,9 @@
       <c r="H78" t="n">
         <v>16778.5</v>
       </c>
+      <c r="I78" t="n">
+        <v>8270.438893832888</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3100,7 +3336,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-0.005786171475387292</v>
+        <v>-0.005786295582733914</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -3126,6 +3362,9 @@
       <c r="H79" t="n">
         <v>16919.39</v>
       </c>
+      <c r="I79" t="n">
+        <v>8339.596275817052</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3134,7 +3373,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.02653643694966945</v>
+        <v>0.02653668554586908</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -3160,6 +3399,9 @@
       <c r="H80" t="n">
         <v>16706.36</v>
       </c>
+      <c r="I80" t="n">
+        <v>8233.926783613717</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3168,7 +3410,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.003266878163248776</v>
+        <v>0.003266878552935282</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -3194,6 +3436,9 @@
       <c r="H81" t="n">
         <v>16547.31</v>
       </c>
+      <c r="I81" t="n">
+        <v>8155.161580167615</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3202,7 +3447,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>-0.02688457456138771</v>
+        <v>-0.02688463897347759</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -3228,6 +3473,9 @@
       <c r="H82" t="n">
         <v>16633.47</v>
       </c>
+      <c r="I82" t="n">
+        <v>8197.514430282616</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3236,7 +3484,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-0.006960505903592207</v>
+        <v>-0.00696056877955975</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -3262,6 +3510,9 @@
       <c r="H83" t="n">
         <v>16607.48</v>
       </c>
+      <c r="I83" t="n">
+        <v>8184.695696554645</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3270,7 +3521,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-0.000912935226457634</v>
+        <v>-0.0009128121504726749</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -3296,6 +3547,9 @@
       <c r="H84" t="n">
         <v>16672.87</v>
       </c>
+      <c r="I84" t="n">
+        <v>8216.858696061214</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3304,7 +3558,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.01401929379191991</v>
+        <v>0.01401929550845082</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -3330,6 +3584,9 @@
       <c r="H85" t="n">
         <v>16675.18</v>
       </c>
+      <c r="I85" t="n">
+        <v>8217.997050095008</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3338,7 +3595,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.002203295387067428</v>
+        <v>0.002203234996217773</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -3364,6 +3621,9 @@
       <c r="H86" t="n">
         <v>16850.36</v>
       </c>
+      <c r="I86" t="n">
+        <v>8303.880339415668</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3372,7 +3632,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>-0.002011392736243067</v>
+        <v>-0.002011271541494608</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -3398,6 +3658,9 @@
       <c r="H87" t="n">
         <v>16831.85</v>
       </c>
+      <c r="I87" t="n">
+        <v>8294.753572463289</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3406,7 +3669,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-0.003383170821594561</v>
+        <v>-0.003383414973788135</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -3432,6 +3695,9 @@
       <c r="H88" t="n">
         <v>16950.65</v>
       </c>
+      <c r="I88" t="n">
+        <v>8353.092699911776</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3440,7 +3706,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.007426738489773044</v>
+        <v>0.007426801281345874</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -3466,6 +3732,9 @@
       <c r="H89" t="n">
         <v>17178.26</v>
       </c>
+      <c r="I89" t="n">
+        <v>8464.510006681468</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3474,7 +3743,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.00961086205642836</v>
+        <v>0.009610924328759651</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -3500,6 +3769,9 @@
       <c r="H90" t="n">
         <v>17440.66</v>
       </c>
+      <c r="I90" t="n">
+        <v>8592.828854414533</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3508,7 +3780,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.0111515721999762</v>
+        <v>0.01115145561185216</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -3534,6 +3806,9 @@
       <c r="H91" t="n">
         <v>17943.26</v>
       </c>
+      <c r="I91" t="n">
+        <v>8836.953658381188</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3542,7 +3817,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.02314686921605613</v>
+        <v>0.02314699186880453</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -3568,6 +3843,9 @@
       <c r="H92" t="n">
         <v>18846.62</v>
       </c>
+      <c r="I92" t="n">
+        <v>9271.016254788028</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3576,7 +3854,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.04101435409019594</v>
+        <v>0.04101413864778891</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -3602,6 +3880,9 @@
       <c r="H93" t="n">
         <v>19930.01</v>
       </c>
+      <c r="I93" t="n">
+        <v>9789.201616049766</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3610,7 +3891,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.0519982827215788</v>
+        <v>0.05199840802272959</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -3636,6 +3917,9 @@
       <c r="H94" t="n">
         <v>21185.65</v>
       </c>
+      <c r="I94" t="n">
+        <v>10387.2966737376</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3644,7 +3928,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.0789961077670025</v>
+        <v>0.07899637171249019</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -3670,6 +3954,9 @@
       <c r="H95" t="n">
         <v>21134.81</v>
       </c>
+      <c r="I95" t="n">
+        <v>10362.33993097392</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3678,7 +3965,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.02685050887141749</v>
+        <v>0.02685041389722898</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -3704,6 +3991,9 @@
       <c r="H96" t="n">
         <v>20677.47</v>
       </c>
+      <c r="I96" t="n">
+        <v>10135.64568942985</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3712,7 +4002,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-0.0217945450436865</v>
+        <v>-0.02179454713632722</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -3738,6 +4028,9 @@
       <c r="H97" t="n">
         <v>21071.59</v>
       </c>
+      <c r="I97" t="n">
+        <v>10327.01667360714</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3746,7 +4039,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0.001688119478952643</v>
+        <v>0.001687925836430182</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -3772,6 +4065,9 @@
       <c r="H98" t="n">
         <v>22667.21</v>
       </c>
+      <c r="I98" t="n">
+        <v>11080.82382124782</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3780,7 +4076,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.05118786792206542</v>
+        <v>0.05118806656375874</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -3806,6 +4102,9 @@
       <c r="H99" t="n">
         <v>22916.45</v>
       </c>
+      <c r="I99" t="n">
+        <v>11201.99935002543</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3814,7 +4113,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.02612394036532173</v>
+        <v>0.02612385304570886</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -3840,6 +4139,9 @@
       <c r="H100" t="n">
         <v>22632.89</v>
       </c>
+      <c r="I100" t="n">
+        <v>11062.52510206675</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3848,7 +4150,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-0.004649657673336804</v>
+        <v>-0.004649568397713466</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -3874,6 +4176,9 @@
       <c r="H101" t="n">
         <v>23060.94</v>
       </c>
+      <c r="I101" t="n">
+        <v>11269.79389059671</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3882,7 +4187,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.01544455995661664</v>
+        <v>0.01544447260704729</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -3908,6 +4213,9 @@
       <c r="H102" t="n">
         <v>23009.65</v>
       </c>
+      <c r="I102" t="n">
+        <v>11244.70074690331</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3916,7 +4224,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.002546163410960034</v>
+        <v>0.002546252367206847</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -3942,6 +4250,9 @@
       <c r="H103" t="n">
         <v>23074.16</v>
       </c>
+      <c r="I103" t="n">
+        <v>11276.18235048604</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3950,7 +4261,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.001479239448809011</v>
+        <v>0.001479327953779475</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -3976,6 +4287,9 @@
       <c r="H104" t="n">
         <v>22826.15</v>
       </c>
+      <c r="I104" t="n">
+        <v>11154.32551767708</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4010,6 +4324,9 @@
       <c r="H105" t="n">
         <v>23125.13</v>
       </c>
+      <c r="I105" t="n">
+        <v>11299.47783137167</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4018,7 +4335,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.003790533836600218</v>
+        <v>0.003790355670405532</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -4044,6 +4361,9 @@
       <c r="H106" t="n">
         <v>23732.66</v>
       </c>
+      <c r="I106" t="n">
+        <v>11592.49875555125</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4052,7 +4372,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.02532921277136602</v>
+        <v>0.02532921722750103</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -4078,6 +4398,9 @@
       <c r="H107" t="n">
         <v>23488.94</v>
       </c>
+      <c r="I107" t="n">
+        <v>11472.83534372035</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4086,7 +4409,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.006712937844120859</v>
+        <v>0.006713025280253859</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -4112,6 +4435,9 @@
       <c r="H108" t="n">
         <v>23431.9</v>
       </c>
+      <c r="I108" t="n">
+        <v>11444.94109245045</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4120,7 +4446,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>-1.07842984551354e-05</v>
+        <v>-1.069802452846602e-05</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -4146,6 +4472,9 @@
       <c r="H109" t="n">
         <v>22762.52</v>
       </c>
+      <c r="I109" t="n">
+        <v>11113.23215696527</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4154,7 +4483,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>-0.02354481091187743</v>
+        <v>-0.02354498757245516</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -4180,6 +4509,9 @@
       <c r="H110" t="n">
         <v>23240.46</v>
       </c>
+      <c r="I110" t="n">
+        <v>11344.15847053906</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4188,7 +4520,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.007100248851111601</v>
+        <v>0.007100425511689323</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -4214,6 +4546,9 @@
       <c r="H111" t="n">
         <v>22963</v>
       </c>
+      <c r="I111" t="n">
+        <v>11207.90945170469</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4222,7 +4557,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>-0.006330570076386266</v>
+        <v>-0.006330658338711714</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -4248,6 +4583,9 @@
       <c r="H112" t="n">
         <v>21796.35</v>
       </c>
+      <c r="I112" t="n">
+        <v>10623.50999549575</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4256,7 +4594,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>-0.04691549639434989</v>
+        <v>-0.04691550063389371</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -4282,6 +4620,9 @@
       <c r="H113" t="n">
         <v>21625.19</v>
       </c>
+      <c r="I113" t="n">
+        <v>10539.75758189733</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4290,7 +4631,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>-0.02466056582232845</v>
+        <v>-0.0246605681318357</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -4316,6 +4657,9 @@
       <c r="H114" t="n">
         <v>21773.97</v>
       </c>
+      <c r="I114" t="n">
+        <v>10612.02217301274</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4324,7 +4668,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>-0.01127486257838761</v>
+        <v>-0.01127476776701108</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -4350,6 +4694,9 @@
       <c r="H115" t="n">
         <v>22199.84</v>
       </c>
+      <c r="I115" t="n">
+        <v>10817.57557780128</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4358,7 +4705,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.02551687949892667</v>
+        <v>0.02551659908697701</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -4384,6 +4731,9 @@
       <c r="H116" t="n">
         <v>24324.05</v>
       </c>
+      <c r="I116" t="n">
+        <v>11806.09094762529</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4392,7 +4742,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.07399954698242439</v>
+        <v>0.07399982739437405</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -4418,6 +4768,9 @@
       <c r="H117" t="n">
         <v>23517.72</v>
       </c>
+      <c r="I117" t="n">
+        <v>11408.09117255898</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4426,7 +4779,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.003319149205207594</v>
+        <v>0.003318976173316557</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -4452,6 +4805,9 @@
       <c r="H118" t="n">
         <v>24569.97</v>
       </c>
+      <c r="I118" t="n">
+        <v>11907.43228965717</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4460,7 +4816,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.03724798878212177</v>
+        <v>0.03724807846133871</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -4486,6 +4842,9 @@
       <c r="H119" t="n">
         <v>24842.2</v>
       </c>
+      <c r="I119" t="n">
+        <v>12038.63855281158</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4494,7 +4853,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.02918862520429499</v>
+        <v>0.02918870855696909</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -4520,6 +4879,9 @@
       <c r="H120" t="n">
         <v>24452.16</v>
       </c>
+      <c r="I120" t="n">
+        <v>11848.12391476877</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -4528,7 +4890,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-0.006449054157652512</v>
+        <v>-0.006449298593647512</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -4554,6 +4916,9 @@
       <c r="H121" t="n">
         <v>24182.21</v>
       </c>
+      <c r="I121" t="n">
+        <v>11716.59413868248</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4562,7 +4927,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-0.02076980487507818</v>
+        <v>-0.02076956043908318</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -4588,6 +4953,9 @@
       <c r="H122" t="n">
         <v>23940.2</v>
       </c>
+      <c r="I122" t="n">
+        <v>11598.74647258775</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -4622,6 +4990,9 @@
       <c r="H123" t="n">
         <v>23185.29</v>
       </c>
+      <c r="I123" t="n">
+        <v>11227.110706742</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -4630,7 +5001,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>-0.02760978466234754</v>
+        <v>-0.02760987068615073</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -4656,6 +5027,9 @@
       <c r="H124" t="n">
         <v>23492.09</v>
       </c>
+      <c r="I124" t="n">
+        <v>11374.69941751335</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -4664,7 +5038,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>-0.00771114980222265</v>
+        <v>-0.007711237157845829</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -4690,6 +5064,9 @@
       <c r="H125" t="n">
         <v>23141.57</v>
       </c>
+      <c r="I125" t="n">
+        <v>11203.70127032875</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -4698,7 +5075,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-0.01213779893365441</v>
+        <v>-0.01213762555422804</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -4724,6 +5101,9 @@
       <c r="H126" t="n">
         <v>23628.97</v>
       </c>
+      <c r="I126" t="n">
+        <v>11437.21927919447</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -4732,7 +5112,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.01898618807683228</v>
+        <v>0.01898610197877915</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
@@ -4758,6 +5138,9 @@
       <c r="H127" t="n">
         <v>23465.32</v>
       </c>
+      <c r="I127" t="n">
+        <v>11357.73157616992</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -4766,7 +5149,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-0.001066893268665936</v>
+        <v>-0.001067065740514295</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -4792,6 +5175,9 @@
       <c r="H128" t="n">
         <v>22354.34</v>
       </c>
+      <c r="I128" t="n">
+        <v>10806.8463763083</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -4800,7 +5186,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-0.03846942590521252</v>
+        <v>-0.03846943604605535</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -4826,6 +5212,9 @@
       <c r="H129" t="n">
         <v>22410</v>
       </c>
+      <c r="I129" t="n">
+        <v>10833.7208652114</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -4834,7 +5223,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-0.01197874757367856</v>
+        <v>-0.01197838821331132</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -4860,6 +5249,9 @@
       <c r="H130" t="n">
         <v>22197.96</v>
       </c>
+      <c r="I130" t="n">
+        <v>10730.72581795771</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -4868,7 +5260,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>-0.008578239863872739</v>
+        <v>-0.008578513374683183</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -4894,6 +5286,9 @@
       <c r="H131" t="n">
         <v>21705.44</v>
       </c>
+      <c r="I131" t="n">
+        <v>10489.95545368007</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4902,7 +5297,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>-0.01601527265553671</v>
+        <v>-0.01601527560768723</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -4928,6 +5323,9 @@
       <c r="H132" t="n">
         <v>20362.22</v>
       </c>
+      <c r="I132" t="n">
+        <v>9819.839294628617</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4936,7 +5334,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>-0.05374447946524263</v>
+        <v>-0.05374448972491663</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -4962,6 +5360,9 @@
       <c r="H133" t="n">
         <v>20150.69</v>
       </c>
+      <c r="I133" t="n">
+        <v>9717.293736563479</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4970,7 +5371,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>-0.02916803256960776</v>
+        <v>-0.02916788696566641</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
@@ -4996,6 +5397,9 @@
       <c r="H134" t="n">
         <v>24113.48</v>
       </c>
+      <c r="I134" t="n">
+        <v>11461.86366979877</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5004,7 +5408,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.108422344282074</v>
+        <v>0.1084222136179278</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
@@ -5030,6 +5434,9 @@
       <c r="H135" t="n">
         <v>24670.41</v>
       </c>
+      <c r="I135" t="n">
+        <v>11723.57847263398</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5038,7 +5445,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.07281837174587125</v>
+        <v>0.07281846867300601</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -5064,6 +5471,9 @@
       <c r="H136" t="n">
         <v>24285.66</v>
       </c>
+      <c r="I136" t="n">
+        <v>11539.30143863778</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5072,7 +5482,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.008590414658550927</v>
+        <v>0.008590415378815663</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
@@ -5098,6 +5508,9 @@
       <c r="H137" t="n">
         <v>24998.78</v>
       </c>
+      <c r="I137" t="n">
+        <v>11873.26002669259</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5106,7 +5519,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.02077650928915098</v>
+        <v>0.02077642923662815</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
@@ -5132,6 +5545,9 @@
       <c r="H138" t="n">
         <v>27395.13</v>
       </c>
+      <c r="I138" t="n">
+        <v>12960.11731333557</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5140,7 +5556,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.06327007006001573</v>
+        <v>0.06327023359835593</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
@@ -5166,6 +5582,9 @@
       <c r="H139" t="n">
         <v>27717.01</v>
       </c>
+      <c r="I139" t="n">
+        <v>13111.50501100754</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5174,7 +5593,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.03191173131500236</v>
+        <v>0.03191158262469784</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
@@ -5200,6 +5619,9 @@
       <c r="H140" t="n">
         <v>28105.47</v>
       </c>
+      <c r="I140" t="n">
+        <v>13293.98982551719</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5208,7 +5630,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.02767672724988657</v>
+        <v>0.02767680362445901</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
@@ -5234,6 +5656,9 @@
       <c r="H141" t="n">
         <v>27250.97</v>
       </c>
+      <c r="I141" t="n">
+        <v>12883.53652687096</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5242,7 +5667,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>-0.01652241871694748</v>
+        <v>-0.01652256696269916</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
@@ -5268,6 +5693,9 @@
       <c r="H142" t="n">
         <v>28295.41</v>
       </c>
+      <c r="I142" t="n">
+        <v>13368.09256968229</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5276,7 +5704,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.01410886355984076</v>
+        <v>0.01410901163084155</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
@@ -5301,6 +5729,9 @@
       </c>
       <c r="H143" t="n">
         <v>27454.47</v>
+      </c>
+      <c r="I143" t="n">
+        <v>12964.76913646107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update model evaluation metrics and predictions accuracy
</commit_message>
<xml_diff>
--- a/data/output/backtest_Close_BTC.xlsx
+++ b/data/output/backtest_Close_BTC.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0006138469469600949</v>
+        <v>0.0006139511933795916</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -561,7 +561,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.06152842560246263</v>
+        <v>0.06152841315326185</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.05214948232460692</v>
+        <v>0.05214928615285963</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -635,7 +635,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.04688672676649652</v>
+        <v>-0.04688653162444112</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.01992836523031372</v>
+        <v>-0.01992861013985703</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.03630076626129508</v>
+        <v>-0.03630056167199491</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.006182425508914235</v>
+        <v>-0.006182424548773824</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -783,7 +783,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.006602968488977012</v>
+        <v>-0.006602915185629499</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.02136562453104141</v>
+        <v>-0.02136562001574127</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.01742764230501948</v>
+        <v>-0.01742774722772289</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -894,7 +894,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.02946957949093765</v>
+        <v>0.02946968185690224</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -931,7 +931,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.02028816482165219</v>
+        <v>0.02028800547912368</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.004594878712980588</v>
+        <v>0.004594878475963071</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1005,7 +1005,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.007962266088021863</v>
+        <v>-0.00796211004945846</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.002646617904192183</v>
+        <v>0.002646513878531209</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1079,7 +1079,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.01477172864263032</v>
+        <v>0.01477182908523034</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1116,7 +1116,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.005116722874085156</v>
+        <v>-0.005116773069479663</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.008906113614404632</v>
+        <v>0.008906010677121046</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.02093297504097436</v>
+        <v>0.02093312319408014</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1227,7 +1227,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.00508627979317211</v>
+        <v>0.005086278783874576</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1264,7 +1264,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.00592431857048048</v>
+        <v>-0.005924217840890478</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.01449278711531932</v>
+        <v>-0.01449288376219471</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1338,7 +1338,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.02739007719521958</v>
+        <v>-0.02739012349140069</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1375,7 +1375,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.004555390384473057</v>
+        <v>-0.004555389673498667</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.002104718545581363</v>
+        <v>0.00210477024987199</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.005994587906439364</v>
+        <v>0.005994534940302998</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.001679560483630382</v>
+        <v>0.001679456952427216</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.01257061021838268</v>
+        <v>0.01257060957335732</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.007766238337204356</v>
+        <v>-0.007766135163812748</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.00858756500723068</v>
+        <v>-0.00858761550875542</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1634,7 +1634,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.00968254594673823</v>
+        <v>-0.009682597273567239</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1671,7 +1671,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.0003146433812766247</v>
+        <v>0.0003147480027134719</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.008503556081565833</v>
+        <v>0.008503606628471161</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.03792210973251109</v>
+        <v>0.03792225184742826</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.03280907582040626</v>
+        <v>0.03280882286863829</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1819,7 +1819,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-0.003937736148355242</v>
+        <v>-0.003937735766957218</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1856,7 +1856,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-0.001792049111680072</v>
+        <v>-0.001791951715237161</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1893,7 +1893,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.000408153491019192</v>
+        <v>0.0004081534116728847</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1930,7 +1930,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-0.01982575703997647</v>
+        <v>-0.01982575314808344</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-0.0191075814639472</v>
+        <v>-0.01910767868027108</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -2004,7 +2004,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-0.005841637504442332</v>
+        <v>-0.005841636912469639</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -2041,7 +2041,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.04350330945818648</v>
+        <v>0.04350320782523909</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -2078,7 +2078,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-0.01385653001977616</v>
+        <v>-0.01385643135569303</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2115,7 +2115,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>-0.07985571145152903</v>
+        <v>-0.07985570324950864</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-0.147797878767463</v>
+        <v>-0.1477979236897742</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2189,7 +2189,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.01421689147663585</v>
+        <v>0.01421707381032178</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2226,7 +2226,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.006356375472220677</v>
+        <v>0.006356252559591269</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-0.009377149964747034</v>
+        <v>-0.009377087567214559</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2300,7 +2300,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.005238368883798472</v>
+        <v>0.005238489791871359</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2337,7 +2337,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-0.02029794064702983</v>
+        <v>-0.02029799658321529</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -2374,7 +2374,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.004536062029579568</v>
+        <v>0.004535999001729962</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -2411,7 +2411,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.005419553176341907</v>
+        <v>0.005419552172616804</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -2448,7 +2448,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.04502589940245727</v>
+        <v>-0.0450257620898924</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2485,7 +2485,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.006819967239302116</v>
+        <v>0.006819837120012551</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -2522,7 +2522,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.02987242721610883</v>
+        <v>0.02987235948570799</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -2559,7 +2559,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.03108308514259939</v>
+        <v>0.0310831415252526</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -2596,7 +2596,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-0.001738685603724477</v>
+        <v>-0.0017387455770006</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -2633,7 +2633,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-0.03353070069447384</v>
+        <v>-0.03353063423974589</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -2670,7 +2670,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-0.009099497097782461</v>
+        <v>-0.009099558301240762</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -2707,7 +2707,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.03510229264497333</v>
+        <v>0.03510253127685203</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -2744,7 +2744,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-0.008120757564272552</v>
+        <v>-0.008120999545745633</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -2781,7 +2781,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.01138770288412871</v>
+        <v>0.01138788313199512</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -2818,7 +2818,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-0.01389573739630023</v>
+        <v>-0.01389591733660467</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -2855,7 +2855,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.004765423454299977</v>
+        <v>0.004765545071014898</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -2892,7 +2892,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>-0.01057497882278291</v>
+        <v>-0.01057509972410031</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2929,7 +2929,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.01599020647839566</v>
+        <v>0.01599008297881532</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2966,7 +2966,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.002902061590788207</v>
+        <v>0.00290230396736213</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -3003,7 +3003,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.01014394761165072</v>
+        <v>0.01014394516542616</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -3040,7 +3040,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.01875378987535825</v>
+        <v>0.01875360881318322</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -3077,7 +3077,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.01331820357692948</v>
+        <v>0.01331837706614714</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -3114,7 +3114,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>-0.01221526921111149</v>
+        <v>-0.01221503114234501</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -3151,7 +3151,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-0.04539433412887739</v>
+        <v>-0.0453946199526527</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-0.02569790395934568</v>
+        <v>-0.02569796228988785</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -3225,7 +3225,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.01941483191194671</v>
+        <v>0.01941489140600972</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -3262,7 +3262,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.007409066324184366</v>
+        <v>0.007408880558280373</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -3299,7 +3299,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.007725413886689125</v>
+        <v>0.007725657854152246</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -3336,7 +3336,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-0.005786295582733914</v>
+        <v>-0.005786171475387292</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -3373,7 +3373,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.02653668554586908</v>
+        <v>0.02653643694966945</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -3410,7 +3410,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.003266878552935282</v>
+        <v>0.003266878163248776</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -3447,7 +3447,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>-0.02688463897347759</v>
+        <v>-0.02688457456138771</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -3484,7 +3484,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-0.00696056877955975</v>
+        <v>-0.006960505903592207</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -3521,7 +3521,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-0.0009128121504726749</v>
+        <v>-0.000912935226457634</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -3558,7 +3558,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.01401929550845082</v>
+        <v>0.01401929379191991</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -3595,7 +3595,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.002203234996217773</v>
+        <v>0.002203295387067428</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>-0.002011271541494608</v>
+        <v>-0.002011392736243067</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -3669,7 +3669,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-0.003383414973788135</v>
+        <v>-0.003383170821594561</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -3706,7 +3706,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.007426801281345874</v>
+        <v>0.007426738489773044</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -3743,7 +3743,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.009610924328759651</v>
+        <v>0.00961086205642836</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -3780,7 +3780,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.01115145561185216</v>
+        <v>0.0111515721999762</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -3817,7 +3817,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.02314699186880453</v>
+        <v>0.02314686921605613</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -3854,7 +3854,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.04101413864778891</v>
+        <v>0.04101435409019594</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -3891,7 +3891,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.05199840802272959</v>
+        <v>0.0519982827215788</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -3928,7 +3928,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.07899637171249019</v>
+        <v>0.0789961077670025</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -3965,7 +3965,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.02685041389722898</v>
+        <v>0.02685050887141749</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -4002,7 +4002,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-0.02179454713632722</v>
+        <v>-0.0217945450436865</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -4039,7 +4039,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0.001687925836430182</v>
+        <v>0.001688119478952643</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -4076,7 +4076,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.05118806656375874</v>
+        <v>0.05118786792206542</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -4113,7 +4113,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.02612385304570886</v>
+        <v>0.02612394036532173</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -4150,7 +4150,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-0.004649568397713466</v>
+        <v>-0.004649657673336804</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -4187,7 +4187,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.01544447260704729</v>
+        <v>0.01544455995661664</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -4224,7 +4224,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.002546252367206847</v>
+        <v>0.002546163410960034</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -4261,7 +4261,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.001479327953779475</v>
+        <v>0.001479239448809011</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -4335,7 +4335,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.003790355670405532</v>
+        <v>0.003790533836600218</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -4372,7 +4372,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.02532921722750103</v>
+        <v>0.02532921277136602</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -4409,7 +4409,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.006713025280253859</v>
+        <v>0.006712937844120859</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -4446,7 +4446,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>-1.069802452846602e-05</v>
+        <v>-1.07842984551354e-05</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -4483,7 +4483,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>-0.02354498757245516</v>
+        <v>-0.02354481091187743</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -4520,7 +4520,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.007100425511689323</v>
+        <v>0.007100248851111601</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -4557,7 +4557,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>-0.006330658338711714</v>
+        <v>-0.006330570076386266</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -4594,7 +4594,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>-0.04691550063389371</v>
+        <v>-0.04691549639434989</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -4631,7 +4631,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>-0.0246605681318357</v>
+        <v>-0.02466056582232845</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -4668,7 +4668,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>-0.01127476776701108</v>
+        <v>-0.01127486257838761</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -4705,7 +4705,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.02551659908697701</v>
+        <v>0.02551687949892667</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -4742,7 +4742,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.07399982739437405</v>
+        <v>0.07399954698242439</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -4779,7 +4779,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.003318976173316557</v>
+        <v>0.003319149205207594</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -4816,7 +4816,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.03724807846133871</v>
+        <v>0.03724798878212177</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -4853,7 +4853,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.02918870855696909</v>
+        <v>0.02918862520429499</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -4890,7 +4890,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-0.006449298593647512</v>
+        <v>-0.006449054157652512</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -4927,7 +4927,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-0.02076956043908318</v>
+        <v>-0.02076980487507818</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -5001,7 +5001,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>-0.02760987068615073</v>
+        <v>-0.02760978466234754</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -5038,7 +5038,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>-0.007711237157845829</v>
+        <v>-0.00771114980222265</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -5075,7 +5075,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-0.01213762555422804</v>
+        <v>-0.01213779893365441</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -5112,7 +5112,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.01898610197877915</v>
+        <v>0.01898618807683228</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
@@ -5149,7 +5149,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-0.001067065740514295</v>
+        <v>-0.001066893268665936</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -5186,7 +5186,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-0.03846943604605535</v>
+        <v>-0.03846942590521252</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -5223,7 +5223,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-0.01197838821331132</v>
+        <v>-0.01197874757367856</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -5260,7 +5260,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>-0.008578513374683183</v>
+        <v>-0.008578239863872739</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -5297,7 +5297,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>-0.01601527560768723</v>
+        <v>-0.01601527265553671</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -5334,7 +5334,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>-0.05374448972491663</v>
+        <v>-0.05374447946524263</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -5371,7 +5371,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>-0.02916788696566641</v>
+        <v>-0.02916803256960776</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
@@ -5408,7 +5408,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.1084222136179278</v>
+        <v>0.108422344282074</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
@@ -5445,7 +5445,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.07281846867300601</v>
+        <v>0.07281837174587125</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -5482,7 +5482,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.008590415378815663</v>
+        <v>0.008590414658550927</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
@@ -5519,7 +5519,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.02077642923662815</v>
+        <v>0.02077650928915098</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
@@ -5556,7 +5556,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.06327023359835593</v>
+        <v>0.06327007006001573</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
@@ -5593,7 +5593,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.03191158262469784</v>
+        <v>0.03191173131500236</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
@@ -5630,7 +5630,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.02767680362445901</v>
+        <v>0.02767672724988657</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
@@ -5667,7 +5667,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>-0.01652256696269916</v>
+        <v>-0.01652241871694748</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
@@ -5704,7 +5704,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.01410901163084155</v>
+        <v>0.01410886355984076</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>

</xml_diff>